<commit_message>
fix: avance de sistema experto
fix: avance de sistema experto
</commit_message>
<xml_diff>
--- a/Proyecto 1/Base de conocimiento.xlsx
+++ b/Proyecto 1/Base de conocimiento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jp_gm\Escritorio\PRIMER SEMESTRE 2022\IA\IA\Laboratorio_IA\Proyecto 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{337902A2-C0A5-4695-967E-157E360F7668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7495622-979A-4E3E-9FB7-23060AA419D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="2" xr2:uid="{EB006548-C89C-4332-8526-5EB2DF5351D6}"/>
   </bookViews>
@@ -2075,7 +2075,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2105,7 +2105,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -2130,7 +2130,7 @@
         <v>departamento(1,peten,8,español,tropical).</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -2230,7 +2230,7 @@
         <v>departamento(5,huehuetenango,7,español,frio).</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -2255,7 +2255,7 @@
         <v>departamento(6,escuintla,2,español,calor).</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -2280,7 +2280,7 @@
         <v>departamento(7,san marcos,3,ingles,calor).</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -2330,7 +2330,7 @@
         <v>departamento(9,baja verapaz,5,ingles,templado).</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -2355,7 +2355,7 @@
         <v>departamento(10,santa rosa,4,ingles,calor).</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -2405,7 +2405,7 @@
         <v>departamento(12,suchitepequez,5,español,templado).</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -2455,7 +2455,7 @@
         <v>departamento(14,guatemala,0,ingles,templado).</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -2480,7 +2480,7 @@
         <v>departamento(15,jalapa,4,ingles,calor).</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -2530,7 +2530,7 @@
         <v>departamento(17,quetzaltenango,3,ingles,frio).</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -2555,7 +2555,7 @@
         <v>departamento(18,el progreso,4,katchikel,calor).</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -2659,7 +2659,7 @@
   <autoFilter ref="A1:E23" xr:uid="{6F61EF10-330E-48DB-BA38-0960F039F5AF}">
     <filterColumn colId="4">
       <filters>
-        <filter val="calor"/>
+        <filter val="tropical"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -2672,11 +2672,12 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
     <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="39.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -3772,7 +3773,7 @@
   <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I44"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>